<commit_message>
Commit 19/12 home, search product, cart
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/Book1.xlsx
+++ b/src/test/resources/testdata/Book1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Tester\Learn testing\Selenium java\JavaSeleniumMavenParallel23\src\test\resources\testdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Tester\Learn testing\TestAutomationFrameworkSelenium-DATN\src\test\resources\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4191EC86-8471-4276-8197-B5A0C48DF790}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA51E259-7726-47C0-9CA1-74E3114FBB02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{7FABECB2-CD6D-4D2C-96D5-0E7B73CD295A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>password</t>
   </si>
@@ -48,6 +48,12 @@
   </si>
   <si>
     <t>admin1@demo.com</t>
+  </si>
+  <si>
+    <t>expected</t>
+  </si>
+  <si>
+    <t>status</t>
   </si>
 </sst>
 </file>
@@ -123,9 +129,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -163,7 +169,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -269,7 +275,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -411,7 +417,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -419,26 +425,34 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CE9FE65-2BFB-4D81-8948-CB27F34B96C4}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>

</xml_diff>